<commit_message>
Finished DAQ and eCVT PCBs rev 2.1. Ready for ordering from JLCPCB
</commit_message>
<xml_diff>
--- a/In Development/PCB Designs/Pin Layout for main DAQ.xlsx
+++ b/In Development/PCB Designs/Pin Layout for main DAQ.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahell\Documents\DAQ\TestCode2020\PCB Designs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahell\Documents\DAQ\In Development\PCB Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBA6BC95-F8FF-4253-8C00-D80A4F5A3016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC87086-0B38-4BDE-8146-7D25B8902FB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AFAD0C13-A868-4B5D-ABDB-FF9BB05C730E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
   <si>
     <t>GND</t>
   </si>
@@ -57,6 +57,63 @@
   </si>
   <si>
     <t>Verse</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>Conn Top</t>
+  </si>
+  <si>
+    <t>Conn Bottom</t>
+  </si>
+  <si>
+    <t>A13 (Brake input)</t>
+  </si>
+  <si>
+    <t>A12 (Brake input)</t>
+  </si>
+  <si>
+    <t>A14 (LDS input)</t>
+  </si>
+  <si>
+    <t>RX2</t>
+  </si>
+  <si>
+    <t>TX2</t>
+  </si>
+  <si>
+    <t>D6 (HE Sensor)</t>
+  </si>
+  <si>
+    <t>D5 (HE Sensor)</t>
   </si>
 </sst>
 </file>
@@ -104,10 +161,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,18 +484,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138CC82B-62F5-44FF-8009-EB632B56FC0F}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="20" width="6.7109375" customWidth="1"/>
+    <col min="1" max="20" width="6.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1</v>
       </c>
@@ -495,131 +557,269 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="N3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="N4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1" t="s">
+      <c r="P4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Daq testing code
</commit_message>
<xml_diff>
--- a/In Development/PCB Designs/Pin Layout for main DAQ.xlsx
+++ b/In Development/PCB Designs/Pin Layout for main DAQ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahell\Documents\DAQ\In Development\PCB Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC87086-0B38-4BDE-8146-7D25B8902FB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DD442A-8FA4-463E-8CC4-214168CC7A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AFAD0C13-A868-4B5D-ABDB-FF9BB05C730E}"/>
+    <workbookView xWindow="1368" yWindow="1368" windowWidth="17280" windowHeight="8916" xr2:uid="{AFAD0C13-A868-4B5D-ABDB-FF9BB05C730E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,11 +165,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,15 +487,15 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="20" width="6.7265625" customWidth="1"/>
+    <col min="1" max="20" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -557,27 +557,27 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -639,7 +639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -701,124 +701,124 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8">
         <v>8</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9">
         <v>4</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="E10">
         <v>3</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>